<commit_message>
Changes in excel Data Retrieval
</commit_message>
<xml_diff>
--- a/src/test/resources/eBayTestData.xlsx
+++ b/src/test/resources/eBayTestData.xlsx
@@ -1,34 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26124"/>
-  <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Downloads/ebayAssaignment/src/test/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18240" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14475" windowHeight="5955"/>
   </bookViews>
   <sheets>
     <sheet name="eBayTestData" sheetId="3" r:id="rId1"/>
     <sheet name="DeviceCapabilities" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="F1:O17"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>TestCase</t>
   </si>
@@ -130,12 +126,15 @@
   </si>
   <si>
     <t>maxPriceRange</t>
+  </si>
+  <si>
+    <t>portNo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -470,26 +469,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="8.83203125" style="3"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -530,7 +530,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -582,22 +582,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -619,8 +619,11 @@
       <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -641,6 +644,9 @@
       </c>
       <c r="G2" t="s">
         <v>18</v>
+      </c>
+      <c r="H2">
+        <v>4723</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final Commit With modifications
</commit_message>
<xml_diff>
--- a/src/test/resources/eBayTestData.xlsx
+++ b/src/test/resources/eBayTestData.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14475" windowHeight="5955" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14475" windowHeight="2310"/>
   </bookViews>
   <sheets>
     <sheet name="eBayTestData" sheetId="3" r:id="rId1"/>
     <sheet name="DeviceCapabilities" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1:H17"/>
+  <oleSize ref="A1:G2"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>eBay_productPurchase</t>
   </si>
@@ -129,6 +129,24 @@
   </si>
   <si>
     <t>TestName</t>
+  </si>
+  <si>
+    <t>invalidUserName</t>
+  </si>
+  <si>
+    <t>invalidPassword</t>
+  </si>
+  <si>
+    <t>automation@gmail.com</t>
+  </si>
+  <si>
+    <t>Testing05</t>
+  </si>
+  <si>
+    <t>Highest Price</t>
+  </si>
+  <si>
+    <t>sortType</t>
   </si>
 </sst>
 </file>
@@ -467,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,9 +505,12 @@
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="8.85546875" style="3"/>
+    <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
@@ -529,8 +550,17 @@
       <c r="M1" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="N1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -569,6 +599,15 @@
       </c>
       <c r="M2">
         <v>100000</v>
+      </c>
+      <c r="N2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -584,7 +623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Implementation of Factory Classes
</commit_message>
<xml_diff>
--- a/src/test/resources/eBayTestData.xlsx
+++ b/src/test/resources/eBayTestData.xlsx
@@ -1,23 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26124"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/git/ebayAutomation/src/test/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="4800"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17920" windowHeight="8400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="eBayTestData" sheetId="3" r:id="rId1"/>
     <sheet name="DeviceCapabilities" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1:G2"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -110,49 +114,49 @@
     <t>NA</t>
   </si>
   <si>
+    <t>8.0.0</t>
+  </si>
+  <si>
+    <t>minPriceRange</t>
+  </si>
+  <si>
+    <t>maxPriceRange</t>
+  </si>
+  <si>
+    <t>portNo</t>
+  </si>
+  <si>
+    <t>TestName</t>
+  </si>
+  <si>
+    <t>invalidUserName</t>
+  </si>
+  <si>
+    <t>invalidPassword</t>
+  </si>
+  <si>
+    <t>automation@gmail.com</t>
+  </si>
+  <si>
+    <t>Testing05</t>
+  </si>
+  <si>
+    <t>sortType</t>
+  </si>
+  <si>
+    <t>Nearest</t>
+  </si>
+  <si>
     <t>ce041604f0a2983204</t>
   </si>
   <si>
-    <t>8.0.0</t>
-  </si>
-  <si>
     <t>samsung</t>
-  </si>
-  <si>
-    <t>minPriceRange</t>
-  </si>
-  <si>
-    <t>maxPriceRange</t>
-  </si>
-  <si>
-    <t>portNo</t>
-  </si>
-  <si>
-    <t>TestName</t>
-  </si>
-  <si>
-    <t>invalidUserName</t>
-  </si>
-  <si>
-    <t>invalidPassword</t>
-  </si>
-  <si>
-    <t>automation@gmail.com</t>
-  </si>
-  <si>
-    <t>Testing05</t>
-  </si>
-  <si>
-    <t>sortType</t>
-  </si>
-  <si>
-    <t>Nearest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -487,32 +491,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="8.85546875" style="3"/>
-    <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="8.83203125" style="3"/>
+    <col min="14" max="14" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
@@ -545,22 +549,22 @@
         <v>24</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -601,13 +605,13 @@
         <v>100000</v>
       </c>
       <c r="N2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" t="s">
         <v>38</v>
-      </c>
-      <c r="P2" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -628,20 +632,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -664,24 +668,24 @@
         <v>9</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>

</xml_diff>